<commit_message>
Reunião Extra - TI
</commit_message>
<xml_diff>
--- a/Arquivos Externos/Relatório Resultado BI - Agosto.xlsx
+++ b/Arquivos Externos/Relatório Resultado BI - Agosto.xlsx
@@ -4,27 +4,29 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr showPivotChartFilter="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="23760" windowHeight="9795" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="23760" windowHeight="9795" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Controle e Reuniões CTI" sheetId="5" r:id="rId1"/>
-    <sheet name="Resumo Contas" sheetId="4" r:id="rId2"/>
-    <sheet name="Contas" sheetId="1" r:id="rId3"/>
-    <sheet name="Solicitações" sheetId="2" r:id="rId4"/>
+    <sheet name="Plan1" sheetId="6" r:id="rId1"/>
+    <sheet name="Controle e Reuniões CTI" sheetId="5" r:id="rId2"/>
+    <sheet name="Resumo Contas" sheetId="4" r:id="rId3"/>
+    <sheet name="Contas" sheetId="1" r:id="rId4"/>
+    <sheet name="Solicitações" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Contas!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Solicitações!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Contas!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Solicitações!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId5"/>
+    <pivotCache cacheId="22" r:id="rId6"/>
+    <pivotCache cacheId="28" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="151">
   <si>
     <t>Valor Total Apresentado da Guia</t>
   </si>
@@ -380,9 +382,6 @@
     <t>Resolvida</t>
   </si>
   <si>
-    <t>Validação</t>
-  </si>
-  <si>
     <t>Contas</t>
   </si>
   <si>
@@ -438,6 +437,48 @@
   </si>
   <si>
     <t>Por Criticidade - TI</t>
+  </si>
+  <si>
+    <t>TI/BI</t>
+  </si>
+  <si>
+    <t>BI</t>
+  </si>
+  <si>
+    <t>Pendente</t>
+  </si>
+  <si>
+    <t>Resolvido</t>
+  </si>
+  <si>
+    <t>Escopo</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Contar de Status</t>
+  </si>
+  <si>
+    <t>Itens</t>
+  </si>
+  <si>
+    <t>Incorretos</t>
+  </si>
+  <si>
+    <t>Corretos</t>
+  </si>
+  <si>
+    <t>Indicadores</t>
+  </si>
+  <si>
+    <t>Não Avaliados</t>
+  </si>
+  <si>
+    <t>Avaliados</t>
   </si>
 </sst>
 </file>
@@ -527,6 +568,356 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Itens</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> Estratégicos - BI - Agosto</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Itens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+            <c:showPercent val="1"/>
+            <c:separator>
+</c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Plan1!$A$13:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Em adamento</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pendente</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Resolvido</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$B$13:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Percentual de</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Indicadores Conferidos</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>BI Contas</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Resumo Contas'!$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Indicadores</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showPercent val="1"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Resumo Contas'!$A$29:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Não Avaliados</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Avaliados</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Resumo Contas'!$B$29:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Itens</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> Estratégicos - TI - Agosto</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Itens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+            <c:showPercent val="1"/>
+            <c:separator>
+</c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Plan1!$A$18:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Em adamento</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pendente</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Resolvido</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$B$18:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000036" footer="0.31496062000000036"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
               <a:rPr lang="en-US"/>
               <a:t>Itens por Status - BI - Agosto</a:t>
             </a:r>
@@ -542,7 +933,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.513779527559025E-3"/>
+          <c:x val="2.5137795275590254E-3"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -580,13 +971,13 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Acompanhamento</c:v>
+                  <c:v>Resolvida</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Em adamento</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Novo</c:v>
+                  <c:v>Em adamento</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Pouco avanço</c:v>
@@ -595,7 +986,7 @@
                   <c:v>Resolvida</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Validação</c:v>
+                  <c:v>Resolvida</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -638,13 +1029,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-BR"/>
   <c:chart>
@@ -673,7 +1064,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.513779527559025E-3"/>
+          <c:x val="2.5137795275590254E-3"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -763,13 +1154,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-BR"/>
   <c:chart>
@@ -798,7 +1189,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.5137795275590258E-3"/>
+          <c:x val="2.5137795275590263E-3"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -888,13 +1279,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000036" footer="0.31496062000000036"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000041" footer="0.31496062000000041"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-BR"/>
   <c:chart>
@@ -923,7 +1314,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.5137795275590271E-3"/>
+          <c:x val="2.5137795275590276E-3"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -1043,13 +1434,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000047" footer="0.31496062000000047"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000052" footer="0.31496062000000052"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-BR"/>
   <c:chart>
@@ -1078,7 +1469,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.5137795275590271E-3"/>
+          <c:x val="2.5137795275590276E-3"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -1150,13 +1541,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000047" footer="0.31496062000000047"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000052" footer="0.31496062000000052"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-BR"/>
   <c:chart>
@@ -1185,7 +1576,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.513779527559028E-3"/>
+          <c:x val="2.5137795275590284E-3"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -1263,19 +1654,15 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000058" footer="0.31496062000000058"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-BR"/>
-  <c:pivotSource>
-    <c:name>[Relatório Resultado BI - Agosto.xlsx]Resumo Contas!Tabela dinâmica1</c:name>
-    <c:fmtId val="0"/>
-  </c:pivotSource>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1287,72 +1674,14 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pt-BR"/>
-              <a:t>Itens</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR"/>
-              <a:t>Avaliados no BI - Contas</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Indicadores Avaliados - BI Contas</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="1.6576334208223961E-2"/>
-          <c:y val="2.777777777777779E-2"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
     </c:title>
-    <c:pivotFmts>
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:layout/>
-          <c:spPr/>
-          <c:txPr>
-            <a:bodyPr/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr/>
-              </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="outEnd"/>
-          <c:showPercent val="1"/>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="1"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="tx2"/>
-          </a:solidFill>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="2"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </c:spPr>
-      </c:pivotFmt>
-    </c:pivotFmts>
     <c:view3D>
       <c:rotX val="30"/>
       <c:perspective val="30"/>
@@ -1366,192 +1695,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Resumo Contas'!$B$3</c:f>
+              <c:f>'Resumo Contas'!$B$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx2"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:spPr/>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showPercent val="1"/>
-            <c:showLeaderLines val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Resumo Contas'!$A$4:$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Não</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sim</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Resumo Contas'!$B$4:$B$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-      </c:pie3DChart>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
-  <c:pivotSource>
-    <c:name>[Relatório Resultado BI - Agosto.xlsx]Resumo Contas!Tabela dinâmica2</c:name>
-    <c:fmtId val="1"/>
-  </c:pivotSource>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Percentual de Avaliados Corretos no BI - Contas</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="9.1565477392249023E-4"/>
-          <c:y val="2.7777777777777776E-2"/>
-        </c:manualLayout>
-      </c:layout>
-    </c:title>
-    <c:pivotFmts>
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:layout/>
-          <c:spPr/>
-          <c:txPr>
-            <a:bodyPr/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr/>
-              </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="outEnd"/>
-          <c:showPercent val="1"/>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="1"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent3">
-              <a:lumMod val="60000"/>
-              <a:lumOff val="40000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="2"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent2">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </c:spPr>
-      </c:pivotFmt>
-    </c:pivotFmts>
-    <c:view3D>
-      <c:rotX val="30"/>
-      <c:perspective val="30"/>
-    </c:view3D>
-    <c:plotArea>
-      <c:layout/>
-      <c:pie3DChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Resumo Contas'!$I$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Total</c:v>
+                  <c:v>Indicadores</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1570,46 +1718,32 @@
             <c:idx val="1"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
           <c:dLbls>
-            <c:spPr/>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
-              </a:p>
-            </c:txPr>
             <c:dLblPos val="outEnd"/>
             <c:showPercent val="1"/>
             <c:showLeaderLines val="1"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Resumo Contas'!$H$5:$H$7</c:f>
+              <c:f>'Resumo Contas'!$A$26:$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Não</c:v>
+                  <c:v>Incorretos</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Sim</c:v>
+                  <c:v>Corretos</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Resumo Contas'!$I$5:$I$7</c:f>
+              <c:f>'Resumo Contas'!$B$26:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1631,15 +1765,85 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1821,27 +2025,66 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 1" descr="Resultado de imagem para planserv">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6905625" y="8086725"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="4" name="Gráfico 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1858,20 +2101,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="5" name="Gráfico 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1918,6 +2161,44 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Padrao2" refreshedDate="43375.616981018517" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="31">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A54:C85" sheet="Controle e Reuniões CTI"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Escopo" numFmtId="0">
+      <sharedItems count="3">
+        <s v="TI/BI"/>
+        <s v="TI"/>
+        <s v="BI"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Area" numFmtId="0">
+      <sharedItems count="10">
+        <s v="Geral"/>
+        <s v="Faturamento"/>
+        <s v="Cadastro"/>
+        <s v="TI"/>
+        <s v="Contas"/>
+        <s v="Regulação"/>
+        <s v="Pagamento"/>
+        <s v="Relacionamento"/>
+        <s v="Gestão"/>
+        <s v="SLA"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Status" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Pendente"/>
+        <s v="Resolvido"/>
+        <s v="Em adamento"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="54">
   <r>
@@ -2247,8 +2528,234 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="31">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="4">
+        <item h="1" x="2"/>
+        <item x="1"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="11">
+        <item x="2"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="8"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="0" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Contar de Status" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica2" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
   <location ref="H4:I7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" showAll="0"/>
@@ -2340,8 +2847,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A3:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" showAll="0"/>
@@ -2699,29 +3206,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W37" sqref="W37"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" s="4">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C85"/>
+  <sheetViews>
+    <sheetView topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:C85"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="5" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>113</v>
+      <c r="A2" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -2736,8 +3374,8 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>115</v>
+      <c r="A4" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2760,8 +3398,8 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>118</v>
+      <c r="A7" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -2769,7 +3407,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
         <v>112</v>
@@ -2817,7 +3455,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B16" t="s">
         <v>112</v>
@@ -2825,7 +3463,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2833,7 +3471,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -2841,7 +3479,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2849,7 +3487,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -2857,7 +3495,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -2865,7 +3503,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
         <v>112</v>
@@ -2873,7 +3511,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -2881,7 +3519,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2889,7 +3527,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2897,7 +3535,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2905,7 +3543,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -2913,7 +3551,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2921,7 +3559,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -2929,7 +3567,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -2937,7 +3575,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B32">
         <v>4</v>
@@ -2945,7 +3583,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -2953,7 +3591,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B35" t="s">
         <v>112</v>
@@ -2961,7 +3599,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B36">
         <v>4</v>
@@ -2969,7 +3607,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -2977,7 +3615,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B39" t="s">
         <v>112</v>
@@ -2985,7 +3623,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B40">
         <v>9</v>
@@ -2993,7 +3631,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B41">
         <v>5</v>
@@ -3001,10 +3639,362 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B42">
         <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>137</v>
+      </c>
+      <c r="B55" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>122</v>
+      </c>
+      <c r="B56" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>122</v>
+      </c>
+      <c r="B57" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>138</v>
+      </c>
+      <c r="B58" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>138</v>
+      </c>
+      <c r="B59" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>122</v>
+      </c>
+      <c r="B60" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>122</v>
+      </c>
+      <c r="B61" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>122</v>
+      </c>
+      <c r="B64" t="s">
+        <v>128</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>138</v>
+      </c>
+      <c r="B65" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>122</v>
+      </c>
+      <c r="B66" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>138</v>
+      </c>
+      <c r="B68" t="s">
+        <v>122</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>122</v>
+      </c>
+      <c r="B69" t="s">
+        <v>129</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>122</v>
+      </c>
+      <c r="B70" t="s">
+        <v>131</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>122</v>
+      </c>
+      <c r="B71" t="s">
+        <v>126</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>137</v>
+      </c>
+      <c r="B72" t="s">
+        <v>120</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>122</v>
+      </c>
+      <c r="B73" t="s">
+        <v>129</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>122</v>
+      </c>
+      <c r="B74" t="s">
+        <v>122</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>122</v>
+      </c>
+      <c r="B75" t="s">
+        <v>129</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>122</v>
+      </c>
+      <c r="B76" t="s">
+        <v>122</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>138</v>
+      </c>
+      <c r="B77" t="s">
+        <v>121</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" t="s">
+        <v>121</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>138</v>
+      </c>
+      <c r="B79" t="s">
+        <v>118</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>138</v>
+      </c>
+      <c r="B80" t="s">
+        <v>119</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>122</v>
+      </c>
+      <c r="B81" t="s">
+        <v>121</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>138</v>
+      </c>
+      <c r="B82" t="s">
+        <v>122</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>122</v>
+      </c>
+      <c r="B83" t="s">
+        <v>122</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>138</v>
+      </c>
+      <c r="B84" t="s">
+        <v>122</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>122</v>
+      </c>
+      <c r="B85" t="s">
+        <v>122</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3013,12 +4003,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:I7"/>
+  <dimension ref="A2:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3096,13 +4086,61 @@
         <v>4</v>
       </c>
     </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B30" s="4">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D55"/>
   <sheetViews>
@@ -3751,7 +4789,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D49"/>
   <sheetViews>

</xml_diff>